<commit_message>
fixed formatting for examples
</commit_message>
<xml_diff>
--- a/src/main/resources/users-guide/sample-data.xlsx
+++ b/src/main/resources/users-guide/sample-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\dynamicpdf-api-samples\excel-conversion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\dynamicpdf-api-samples\excel-word-conversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7681A9BB-54DA-4941-9C22-CD14BFF45332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3D5B4B-B6BE-4133-A721-C194A544C35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="6105" windowWidth="43200" windowHeight="23985" xr2:uid="{CE120CA2-B4E2-4FC9-9B81-FB00098FDFE6}"/>
+    <workbookView xWindow="2925" yWindow="855" windowWidth="21600" windowHeight="13980" xr2:uid="{CE120CA2-B4E2-4FC9-9B81-FB00098FDFE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Management Data" sheetId="2" r:id="rId1"/>
@@ -486,13 +486,7 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -504,6 +498,12 @@
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -843,1126 +843,1131 @@
   <dimension ref="B2:H52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="6" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>45292</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>13</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <v>45305</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <v>0.78</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>45305</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>14</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <v>45319</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>45319</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>22</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <v>45341</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <v>0.45</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="4">
         <v>45340</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>25</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="4">
         <v>45365</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <v>45293</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>18</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="4">
         <v>45311</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>45311</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>10</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <v>45321</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <v>0.78</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="4">
         <v>45326</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
         <v>25</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="4">
         <v>45351</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="4">
         <v>45323</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="3">
         <v>22</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="4">
         <v>45345</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="4">
         <v>45346</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="3">
         <v>25</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="4">
         <v>45371</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="4">
         <v>45372</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="3">
         <v>30</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="4">
         <v>45402</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="4">
         <v>45324</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="3">
         <v>22</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="4">
         <v>45346</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="5">
         <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="4">
         <v>45335</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="3">
         <v>21</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="4">
         <v>45331</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="5">
         <v>0.78</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="4">
         <v>45370</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="3">
         <v>25</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="4">
         <v>45395</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="4">
         <v>45293</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="3">
         <v>23</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="4">
         <v>45316</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="5">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="4">
         <v>45317</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="3">
         <v>32</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="4">
         <v>45349</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="4">
         <v>45350</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="3">
         <v>27</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="4">
         <v>45377</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="4">
         <v>45293</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="3">
         <v>36</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="4">
         <v>45329</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="4">
         <v>45330</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="3">
         <v>34</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="4">
         <v>45364</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="4">
         <v>45365</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="3">
         <v>30</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="4">
         <v>45395</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="4">
         <v>45294</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="3">
         <v>47</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="4">
         <v>45341</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="5">
         <v>0.3</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="4">
         <v>45339</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="3">
         <v>27</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="4">
         <v>45366</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="4">
         <v>45365</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="3">
         <v>22</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="4">
         <v>45387</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="4">
         <v>45294</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="3">
         <v>60</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="4">
         <v>45354</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="5">
         <v>0.7</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="4">
         <v>45297</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="3">
         <v>20</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="4">
         <v>45317</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="5">
         <v>0.78</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="4">
         <v>45325</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="3">
         <v>35</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="4">
         <v>45360</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="4">
         <v>45292</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="3">
         <v>25</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="4">
         <v>45317</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="4">
         <v>45318</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="3">
         <v>31</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="4">
         <v>45349</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="4">
         <v>45353</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F34" s="3">
         <v>22</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="4">
         <v>45375</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="4">
         <v>45294</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="3">
         <v>30</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="4">
         <v>45324</v>
       </c>
-      <c r="H35" s="7">
+      <c r="H35" s="5">
         <v>0.4</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="4">
         <v>45325</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="3">
         <v>25</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36" s="4">
         <v>45350</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="4">
         <v>45351</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="3">
         <v>20</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37" s="4">
         <v>45371</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="4">
         <v>45293</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="3">
         <v>35</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="4">
         <v>45328</v>
       </c>
-      <c r="H38" s="7">
+      <c r="H38" s="5">
         <v>0.6</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="4">
         <v>45324</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F39" s="3">
         <v>32</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G39" s="4">
         <v>45356</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="4">
         <v>45357</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="3">
         <v>25</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="4">
         <v>45382</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="4">
         <v>45295</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="3">
         <v>27</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41" s="4">
         <v>45322</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="5">
         <v>0.8</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="4">
         <v>45319</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="3">
         <v>30</v>
       </c>
-      <c r="G42" s="6">
+      <c r="G42" s="4">
         <v>45349</v>
       </c>
-      <c r="H42" s="7">
+      <c r="H42" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="4">
         <v>45350</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="3">
         <v>22</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="4">
         <v>45372</v>
       </c>
-      <c r="H43" s="7">
+      <c r="H43" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="4">
         <v>45294</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F44" s="3">
         <v>25</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="4">
         <v>45319</v>
       </c>
-      <c r="H44" s="7">
+      <c r="H44" s="5">
         <v>0.3</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="4">
         <v>45325</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="3">
         <v>20</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45" s="4">
         <v>45345</v>
       </c>
-      <c r="H45" s="7">
+      <c r="H45" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="4">
         <v>45346</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F46" s="3">
         <v>35</v>
       </c>
-      <c r="G46" s="6">
+      <c r="G46" s="4">
         <v>45381</v>
       </c>
-      <c r="H46" s="7">
+      <c r="H46" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="4">
         <v>45294</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="3">
         <v>25</v>
       </c>
-      <c r="G47" s="6">
+      <c r="G47" s="4">
         <v>45319</v>
       </c>
-      <c r="H47" s="7">
+      <c r="H47" s="5">
         <v>0.5</v>
       </c>
     </row>
     <row r="48" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="4">
         <v>45320</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="3">
         <v>30</v>
       </c>
-      <c r="G48" s="6">
+      <c r="G48" s="4">
         <v>45350</v>
       </c>
-      <c r="H48" s="7">
+      <c r="H48" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="4">
         <v>45380</v>
       </c>
-      <c r="F49" s="5">
+      <c r="F49" s="3">
         <v>20</v>
       </c>
-      <c r="G49" s="6">
+      <c r="G49" s="4">
         <v>45400</v>
       </c>
-      <c r="H49" s="7">
+      <c r="H49" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="4">
         <v>45293</v>
       </c>
-      <c r="F50" s="5">
+      <c r="F50" s="3">
         <v>25</v>
       </c>
-      <c r="G50" s="6">
+      <c r="G50" s="4">
         <v>45318</v>
       </c>
-      <c r="H50" s="7">
+      <c r="H50" s="5">
         <v>0.2</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51" s="4">
         <v>45324</v>
       </c>
-      <c r="F51" s="5">
+      <c r="F51" s="3">
         <v>22</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G51" s="4">
         <v>45346</v>
       </c>
-      <c r="H51" s="7">
+      <c r="H51" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="4">
         <v>45345</v>
       </c>
-      <c r="F52" s="5">
+      <c r="F52" s="3">
         <v>27</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G52" s="4">
         <v>45372</v>
       </c>
-      <c r="H52" s="7">
+      <c r="H52" s="5">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>